<commit_message>
fixes and even more experiments
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/be52199d604fa2c0/Documents/Uni/25 SS/xAI-Proj/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="223" documentId="8_{633C34D0-72DC-407B-B8DA-0E127AFD5C28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90CD1A1B-EE25-4559-ADF8-4BC423BDA863}"/>
+  <xr:revisionPtr revIDLastSave="251" documentId="8_{633C34D0-72DC-407B-B8DA-0E127AFD5C28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1496798F-0B77-46FA-896C-EBD054EFAADD}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="374">
   <si>
     <t>Optimizer</t>
   </si>
@@ -1093,6 +1093,60 @@
   </si>
   <si>
     <t>total: 0.6884, std: 0.0102</t>
+  </si>
+  <si>
+    <t>art painting: 0.8698, std: 0.0069</t>
+  </si>
+  <si>
+    <t>cartoon: 0.7587, std: 0.0095</t>
+  </si>
+  <si>
+    <t>photo: 0.9800, std: 0.0022</t>
+  </si>
+  <si>
+    <t>sketch: 0.7413, std: 0.0224</t>
+  </si>
+  <si>
+    <t>total: 0.8374, std: 0.0016</t>
+  </si>
+  <si>
+    <t>photo: 0.9772</t>
+  </si>
+  <si>
+    <t>sketch: 0.7097</t>
+  </si>
+  <si>
+    <t>total: 0.7376, std: 0.0200</t>
+  </si>
+  <si>
+    <t>resnet50_ms12_a0d1</t>
+  </si>
+  <si>
+    <t>art painting: 0.8988, std: 0.0027</t>
+  </si>
+  <si>
+    <t>cartoon: 0.7651, std: 0.0051</t>
+  </si>
+  <si>
+    <t>photo: 0.9794, std: 0.0028</t>
+  </si>
+  <si>
+    <t>sketch: 0.7204, std: 0.0206</t>
+  </si>
+  <si>
+    <t>total: 0.8409, std: 0.0044</t>
+  </si>
+  <si>
+    <t>art painting: 0.8960</t>
+  </si>
+  <si>
+    <t>cartoon: 0.7607</t>
+  </si>
+  <si>
+    <t>sketch: 0.7041</t>
+  </si>
+  <si>
+    <t>total: 0.7204, std: 0.0206</t>
   </si>
 </sst>
 </file>
@@ -1611,10 +1665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G289"/>
+  <dimension ref="A1:G299"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A263" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C289" sqref="C289"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1622,7 +1676,7 @@
     <col min="1" max="1" width="48" customWidth="1"/>
     <col min="2" max="2" width="36.7109375" customWidth="1"/>
     <col min="3" max="3" width="93" customWidth="1"/>
-    <col min="5" max="5" width="27" customWidth="1"/>
+    <col min="5" max="5" width="33.5703125" customWidth="1"/>
     <col min="6" max="6" width="33.42578125" customWidth="1"/>
     <col min="7" max="7" width="59" customWidth="1"/>
   </cols>
@@ -1901,6 +1955,9 @@
       <c r="C18" t="s">
         <v>38</v>
       </c>
+      <c r="E18" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -4104,43 +4161,43 @@
       <c r="A280" t="s">
         <v>336</v>
       </c>
-      <c r="B280" s="22" t="s">
+      <c r="B280" t="s">
         <v>337</v>
       </c>
-      <c r="C280" s="22" t="s">
+      <c r="C280" t="s">
         <v>342</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B281" s="22" t="s">
+      <c r="B281" t="s">
         <v>338</v>
       </c>
-      <c r="C281" s="22" t="s">
+      <c r="C281" t="s">
         <v>343</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B282" s="22" t="s">
+      <c r="B282" t="s">
         <v>339</v>
       </c>
-      <c r="C282" s="22" t="s">
+      <c r="C282" t="s">
         <v>344</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B283" s="22" t="s">
+      <c r="B283" t="s">
         <v>340</v>
       </c>
-      <c r="C283" s="22" t="s">
+      <c r="C283" t="s">
         <v>345</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A284" s="16"/>
-      <c r="B284" s="23" t="s">
+      <c r="B284" s="16" t="s">
         <v>341</v>
       </c>
-      <c r="C284" s="23" t="s">
+      <c r="C284" s="16" t="s">
         <v>346</v>
       </c>
     </row>
@@ -4148,43 +4205,131 @@
       <c r="A285" t="s">
         <v>347</v>
       </c>
-      <c r="B285" s="22" t="s">
+      <c r="B285" t="s">
         <v>348</v>
       </c>
-      <c r="C285" s="22" t="s">
+      <c r="C285" t="s">
         <v>352</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B286" s="22" t="s">
+      <c r="B286" t="s">
         <v>349</v>
       </c>
-      <c r="C286" s="22" t="s">
+      <c r="C286" t="s">
         <v>353</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B287" s="22" t="s">
+      <c r="B287" t="s">
         <v>266</v>
       </c>
-      <c r="C287" s="22" t="s">
+      <c r="C287" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B288" s="22" t="s">
+      <c r="B288" t="s">
         <v>350</v>
       </c>
-      <c r="C288" s="22" t="s">
+      <c r="C288" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="289" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B289" s="22" t="s">
+    <row r="289" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A289" s="16"/>
+      <c r="B289" s="16" t="s">
         <v>351</v>
       </c>
-      <c r="C289" s="22" t="s">
+      <c r="C289" s="16" t="s">
         <v>355</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A290" t="s">
+        <v>32</v>
+      </c>
+      <c r="B290" s="22" t="s">
+        <v>356</v>
+      </c>
+      <c r="C290" s="22" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B291" s="22" t="s">
+        <v>357</v>
+      </c>
+      <c r="C291" s="22" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B292" s="22" t="s">
+        <v>358</v>
+      </c>
+      <c r="C292" s="22" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B293" s="22" t="s">
+        <v>359</v>
+      </c>
+      <c r="C293" s="22" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A294" s="16"/>
+      <c r="B294" s="23" t="s">
+        <v>360</v>
+      </c>
+      <c r="C294" s="23" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A295" t="s">
+        <v>364</v>
+      </c>
+      <c r="B295" s="22" t="s">
+        <v>365</v>
+      </c>
+      <c r="C295" s="22" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B296" s="22" t="s">
+        <v>366</v>
+      </c>
+      <c r="C296" s="22" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B297" s="22" t="s">
+        <v>367</v>
+      </c>
+      <c r="C297" s="22" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B298" s="22" t="s">
+        <v>368</v>
+      </c>
+      <c r="C298" s="22" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B299" s="22" t="s">
+        <v>369</v>
+      </c>
+      <c r="C299" s="22" t="s">
+        <v>373</v>
       </c>
     </row>
   </sheetData>

</xml_diff>